<commit_message>
run dist commute model, all-city models for distagg and distcomm
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/dist_commute/All.xlsx
+++ b/outputs/ML_Results/dist_commute/All.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ31109471" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ52855637" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ10042081" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ18038994" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ26374957" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ34669728" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ42575960" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ50296179" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ59261357" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ15521233" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ26595024" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ36978498" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ46876033" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ56495105" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ06128269" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ15792861" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ25115217" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ37004755" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -466,10 +466,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9938.795605283838</v>
+        <v>11243.79617795625</v>
       </c>
       <c r="C2" t="n">
-        <v>1.224225704838073e-275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -479,10 +479,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1254.703767228016</v>
+        <v>-1087.598754232779</v>
       </c>
       <c r="C3" t="n">
-        <v>2.335874823484993e-24</v>
+        <v>7.883062979730674e-17</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-703.2295690541619</v>
+        <v>-629.9934058528731</v>
       </c>
       <c r="C4" t="n">
-        <v>1.731241452031001e-20</v>
+        <v>4.661414354048255e-15</v>
       </c>
     </row>
     <row r="5">
@@ -505,10 +505,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-157.3691123613295</v>
+        <v>-42.34593634253093</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02251342680584754</v>
+        <v>0.5615324586307419</v>
       </c>
     </row>
     <row r="6">
@@ -518,10 +518,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.295162579489244</v>
+        <v>0.9772999840473346</v>
       </c>
       <c r="C6" t="n">
-        <v>0.90131735840258</v>
+        <v>0.99017650071507</v>
       </c>
     </row>
     <row r="7">
@@ -531,10 +531,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-103.1195910945912</v>
+        <v>-108.4515537124643</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3026196117157076</v>
+        <v>0.2997803427196951</v>
       </c>
     </row>
     <row r="8">
@@ -544,10 +544,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-347.8055016689519</v>
+        <v>-184.4369065427579</v>
       </c>
       <c r="C8" t="n">
-        <v>5.673719818057806e-07</v>
+        <v>0.01225590129741722</v>
       </c>
     </row>
     <row r="9">
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1875.130426192851</v>
+        <v>-2033.315999996755</v>
       </c>
       <c r="C9" t="n">
-        <v>9.660031398860104e-47</v>
+        <v>3.175313032356555e-49</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1135.626567512023</v>
+        <v>-300.4052064396601</v>
       </c>
       <c r="C10" t="n">
-        <v>2.157899392643272e-18</v>
+        <v>0.02811004747364284</v>
       </c>
     </row>
     <row r="11">
@@ -583,10 +583,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1729.323623488715</v>
+        <v>-2035.188848360659</v>
       </c>
       <c r="C11" t="n">
-        <v>7.395782092333521e-35</v>
+        <v>8.304832608342858e-43</v>
       </c>
     </row>
     <row r="12">
@@ -596,10 +596,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>23.22027852615415</v>
+        <v>36.90557870749245</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1779494322188193</v>
+        <v>0.04374053330405612</v>
       </c>
     </row>
     <row r="13">
@@ -609,10 +609,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1197.18799065438</v>
+        <v>-1414.938816026212</v>
       </c>
       <c r="C13" t="n">
-        <v>4.433261056811779e-179</v>
+        <v>1.922701840137425e-221</v>
       </c>
     </row>
     <row r="14">
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-17.2342985959741</v>
+        <v>-21.62990845618092</v>
       </c>
       <c r="C14" t="n">
-        <v>9.2653713751497e-22</v>
+        <v>9.741292580234047e-30</v>
       </c>
     </row>
     <row r="15">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>153.5713738796453</v>
+        <v>166.6146120143258</v>
       </c>
       <c r="C15" t="n">
-        <v>2.518772616220652e-46</v>
+        <v>1.172369748120113e-47</v>
       </c>
     </row>
     <row r="16">
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>370.3834907817185</v>
+        <v>355.2483789869609</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.02090443924324253</v>
+        <v>-0.01187159471277329</v>
       </c>
       <c r="C17" t="n">
-        <v>3.604962056457423e-09</v>
+        <v>0.001479231848008887</v>
       </c>
     </row>
     <row r="18">
@@ -674,10 +674,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-4.079070143201705e-06</v>
+        <v>-5.081232512475589e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1065438271975032</v>
+        <v>0.06037113129569731</v>
       </c>
     </row>
     <row r="19">
@@ -687,10 +687,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-13.30525913391522</v>
+        <v>-14.20001850220658</v>
       </c>
       <c r="C19" t="n">
-        <v>6.452932389450499e-26</v>
+        <v>4.719000756605821e-26</v>
       </c>
     </row>
     <row r="20">
@@ -700,10 +700,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>7.851232998569001</v>
+        <v>1.894324955612224</v>
       </c>
       <c r="C20" t="n">
-        <v>7.474471485990711e-08</v>
+        <v>0.2169200857165875</v>
       </c>
     </row>
     <row r="21">
@@ -713,10 +713,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3257.169255851396</v>
+        <v>-3410.987900042473</v>
       </c>
       <c r="C21" t="n">
-        <v>3.638275087240003e-50</v>
+        <v>5.910283370008218e-49</v>
       </c>
     </row>
     <row r="22">
@@ -726,10 +726,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1540.790912776203</v>
+        <v>-2106.987318221406</v>
       </c>
       <c r="C22" t="n">
-        <v>1.917351919317249e-23</v>
+        <v>1.314138304204614e-37</v>
       </c>
     </row>
   </sheetData>
@@ -775,10 +775,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10061.92562230057</v>
+        <v>11167.98468632668</v>
       </c>
       <c r="C2" t="n">
-        <v>3.363339697617669e-285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -788,10 +788,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1188.107770087815</v>
+        <v>-1122.479929898641</v>
       </c>
       <c r="C3" t="n">
-        <v>2.643433605304189e-22</v>
+        <v>7.472379288695435e-18</v>
       </c>
     </row>
     <row r="4">
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-658.5722894521861</v>
+        <v>-605.8827068638119</v>
       </c>
       <c r="C4" t="n">
-        <v>2.642157538669037e-18</v>
+        <v>4.895991359053396e-14</v>
       </c>
     </row>
     <row r="5">
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-160.3911872564842</v>
+        <v>-3.950320892034341</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01942437722162388</v>
+        <v>0.9568000532603806</v>
       </c>
     </row>
     <row r="6">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-57.28242484211971</v>
+        <v>103.0508486883163</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4432649998631367</v>
+        <v>0.1941131675007856</v>
       </c>
     </row>
     <row r="7">
@@ -840,10 +840,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-248.2184580305279</v>
+        <v>82.74115545392959</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01287186341317309</v>
+        <v>0.4301430866021332</v>
       </c>
     </row>
     <row r="8">
@@ -853,10 +853,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-399.1522589070919</v>
+        <v>-126.1428649277336</v>
       </c>
       <c r="C8" t="n">
-        <v>7.960626186484467e-09</v>
+        <v>0.08668968115923678</v>
       </c>
     </row>
     <row r="9">
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1876.201852720203</v>
+        <v>-2171.699485444579</v>
       </c>
       <c r="C9" t="n">
-        <v>4.708945481871167e-47</v>
+        <v>3.977909449446567e-56</v>
       </c>
     </row>
     <row r="10">
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1122.005408120902</v>
+        <v>-390.5458239227846</v>
       </c>
       <c r="C10" t="n">
-        <v>5.076995996153763e-18</v>
+        <v>0.004252762555056547</v>
       </c>
     </row>
     <row r="11">
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1721.68633968106</v>
+        <v>-2253.757367990875</v>
       </c>
       <c r="C11" t="n">
-        <v>9.84739694215983e-35</v>
+        <v>3.249861634128237e-52</v>
       </c>
     </row>
     <row r="12">
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>12.40499840836703</v>
+        <v>39.65216240601684</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4709800466496585</v>
+        <v>0.03053267750596244</v>
       </c>
     </row>
     <row r="13">
@@ -918,10 +918,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1169.62817658538</v>
+        <v>-1350.29074465339</v>
       </c>
       <c r="C13" t="n">
-        <v>5.04276205423183e-172</v>
+        <v>4.375213873407448e-202</v>
       </c>
     </row>
     <row r="14">
@@ -931,10 +931,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-19.36069536666152</v>
+        <v>-21.18380653585208</v>
       </c>
       <c r="C14" t="n">
-        <v>3.226206678279638e-27</v>
+        <v>1.039425638206705e-28</v>
       </c>
     </row>
     <row r="15">
@@ -944,10 +944,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>147.031126181087</v>
+        <v>156.861753166799</v>
       </c>
       <c r="C15" t="n">
-        <v>1.468903181863129e-42</v>
+        <v>1.633926226383182e-42</v>
       </c>
     </row>
     <row r="16">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>368.3338796395998</v>
+        <v>359.0706880204943</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -970,10 +970,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.02016523943325712</v>
+        <v>-0.01187988037484579</v>
       </c>
       <c r="C17" t="n">
-        <v>1.129632385672543e-08</v>
+        <v>0.001423213129402359</v>
       </c>
     </row>
     <row r="18">
@@ -983,10 +983,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-3.870378664437671e-06</v>
+        <v>-4.997248222161392e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1203705623262463</v>
+        <v>0.06448324112343772</v>
       </c>
     </row>
     <row r="19">
@@ -996,10 +996,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-13.50673298605259</v>
+        <v>-13.76845334144969</v>
       </c>
       <c r="C19" t="n">
-        <v>1.139535786498514e-26</v>
+        <v>1.169728722237916e-24</v>
       </c>
     </row>
     <row r="20">
@@ -1009,10 +1009,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>8.340326100888436</v>
+        <v>2.007932097422392</v>
       </c>
       <c r="C20" t="n">
-        <v>7.971443830772303e-09</v>
+        <v>0.1904980096653297</v>
       </c>
     </row>
     <row r="21">
@@ -1022,10 +1022,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3305.904227522195</v>
+        <v>-3357.273591625128</v>
       </c>
       <c r="C21" t="n">
-        <v>9.896670158967037e-52</v>
+        <v>1.81918983533962e-47</v>
       </c>
     </row>
     <row r="22">
@@ -1035,10 +1035,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1522.192862729138</v>
+        <v>-2079.798905065328</v>
       </c>
       <c r="C22" t="n">
-        <v>3.859326861321577e-23</v>
+        <v>1.198957241735693e-36</v>
       </c>
     </row>
   </sheetData>
@@ -1084,10 +1084,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9824.241762039725</v>
+        <v>11196.65944754439</v>
       </c>
       <c r="C2" t="n">
-        <v>8.865943085101285e-272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1246.209359447103</v>
+        <v>-1214.890343121068</v>
       </c>
       <c r="C3" t="n">
-        <v>3.645686392888596e-24</v>
+        <v>1.433107935373933e-20</v>
       </c>
     </row>
     <row r="4">
@@ -1110,10 +1110,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-709.4041123876605</v>
+        <v>-650.5175456772636</v>
       </c>
       <c r="C4" t="n">
-        <v>6.677510798724232e-21</v>
+        <v>7.364032164292536e-16</v>
       </c>
     </row>
     <row r="5">
@@ -1123,10 +1123,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-175.3960232722384</v>
+        <v>-45.04274703866662</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01078606801886631</v>
+        <v>0.5385342137254314</v>
       </c>
     </row>
     <row r="6">
@@ -1136,10 +1136,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-26.74105906517642</v>
+        <v>30.92506125994994</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7210705538375415</v>
+        <v>0.6964678350856206</v>
       </c>
     </row>
     <row r="7">
@@ -1149,10 +1149,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-85.02808384800522</v>
+        <v>-78.29582830820775</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3943946372107002</v>
+        <v>0.4550989805004411</v>
       </c>
     </row>
     <row r="8">
@@ -1162,10 +1162,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-351.6855706888036</v>
+        <v>-141.4086850194992</v>
       </c>
       <c r="C8" t="n">
-        <v>4.053176862223239e-07</v>
+        <v>0.0544480447071491</v>
       </c>
     </row>
     <row r="9">
@@ -1175,10 +1175,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1800.923585275372</v>
+        <v>-1965.134976963956</v>
       </c>
       <c r="C9" t="n">
-        <v>1.427856282729574e-43</v>
+        <v>5.827477726395934e-46</v>
       </c>
     </row>
     <row r="10">
@@ -1188,10 +1188,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1083.757137726821</v>
+        <v>-189.7349855820648</v>
       </c>
       <c r="C10" t="n">
-        <v>5.631694975438541e-17</v>
+        <v>0.1664333349633761</v>
       </c>
     </row>
     <row r="11">
@@ -1201,10 +1201,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1641.677182424985</v>
+        <v>-2049.562123671228</v>
       </c>
       <c r="C11" t="n">
-        <v>9.337351696877608e-32</v>
+        <v>2.547849399657772e-43</v>
       </c>
     </row>
     <row r="12">
@@ -1214,10 +1214,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>33.77131138447079</v>
+        <v>42.82660120582686</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0507909921133675</v>
+        <v>0.01924861677819146</v>
       </c>
     </row>
     <row r="13">
@@ -1227,10 +1227,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1151.407287414698</v>
+        <v>-1404.176206088445</v>
       </c>
       <c r="C13" t="n">
-        <v>1.984908166519042e-166</v>
+        <v>2.855783499683493e-218</v>
       </c>
     </row>
     <row r="14">
@@ -1240,10 +1240,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-18.81954343528526</v>
+        <v>-21.3315035211351</v>
       </c>
       <c r="C14" t="n">
-        <v>1.037172787170075e-25</v>
+        <v>5.310207318212908e-29</v>
       </c>
     </row>
     <row r="15">
@@ -1253,10 +1253,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>149.348141856133</v>
+        <v>160.5347389763042</v>
       </c>
       <c r="C15" t="n">
-        <v>8.933061604413637e-44</v>
+        <v>2.329676958382297e-44</v>
       </c>
     </row>
     <row r="16">
@@ -1266,7 +1266,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>365.2721867898842</v>
+        <v>357.9186042813694</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -1279,10 +1279,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.01774325248008451</v>
+        <v>-0.009675315488275021</v>
       </c>
       <c r="C17" t="n">
-        <v>4.827559977320164e-07</v>
+        <v>0.009531414117897574</v>
       </c>
     </row>
     <row r="18">
@@ -1292,10 +1292,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-6.465731373162223e-06</v>
+        <v>-6.441339631744781e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01009780323660053</v>
+        <v>0.0176242854565849</v>
       </c>
     </row>
     <row r="19">
@@ -1305,10 +1305,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-13.18789369418872</v>
+        <v>-13.72713222903662</v>
       </c>
       <c r="C19" t="n">
-        <v>1.198860163426627e-25</v>
+        <v>2.43923960061793e-24</v>
       </c>
     </row>
     <row r="20">
@@ -1318,10 +1318,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>9.184903170814563</v>
+        <v>1.42139707096741</v>
       </c>
       <c r="C20" t="n">
-        <v>2.16873036942023e-10</v>
+        <v>0.3551017723666504</v>
       </c>
     </row>
     <row r="21">
@@ -1331,10 +1331,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3415.087385440362</v>
+        <v>-3490.729181506121</v>
       </c>
       <c r="C21" t="n">
-        <v>3.459974690315021e-55</v>
+        <v>2.487218677973828e-51</v>
       </c>
     </row>
     <row r="22">
@@ -1344,10 +1344,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1549.309552703999</v>
+        <v>-2229.641190644832</v>
       </c>
       <c r="C22" t="n">
-        <v>6.786530378994551e-24</v>
+        <v>6.813677194858813e-42</v>
       </c>
     </row>
   </sheetData>
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10214.96113395667</v>
+        <v>11237.66856428766</v>
       </c>
       <c r="C2" t="n">
-        <v>7.846928544308505e-293</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1406,10 +1406,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1243.429612362447</v>
+        <v>-1002.703640651659</v>
       </c>
       <c r="C3" t="n">
-        <v>4.164917254598491e-24</v>
+        <v>3.312204593778047e-14</v>
       </c>
     </row>
     <row r="4">
@@ -1419,10 +1419,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-760.0828540393359</v>
+        <v>-609.5513655827401</v>
       </c>
       <c r="C4" t="n">
-        <v>7.832375032060267e-24</v>
+        <v>3.915127005584314e-14</v>
       </c>
     </row>
     <row r="5">
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-187.4720213689097</v>
+        <v>-36.23670045552715</v>
       </c>
       <c r="C5" t="n">
-        <v>0.006337722615724841</v>
+        <v>0.6206119956802914</v>
       </c>
     </row>
     <row r="6">
@@ -1445,10 +1445,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>87.48833475953074</v>
+        <v>165.2325015926298</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2422408827684002</v>
+        <v>0.03733551049862015</v>
       </c>
     </row>
     <row r="7">
@@ -1458,10 +1458,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-72.0108485415908</v>
+        <v>50.30729164457304</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4703394278614996</v>
+        <v>0.6303050838627869</v>
       </c>
     </row>
     <row r="8">
@@ -1471,10 +1471,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-253.68706185225</v>
+        <v>-69.9197973945824</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0002524024755669333</v>
+        <v>0.3422919759453927</v>
       </c>
     </row>
     <row r="9">
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1917.161149051576</v>
+        <v>-2191.452775428934</v>
       </c>
       <c r="C9" t="n">
-        <v>2.076850807411006e-49</v>
+        <v>4.922113825468657e-57</v>
       </c>
     </row>
     <row r="10">
@@ -1497,10 +1497,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1159.501928585041</v>
+        <v>-430.9084380999921</v>
       </c>
       <c r="C10" t="n">
-        <v>2.665996977122483e-19</v>
+        <v>0.0016216094225466</v>
       </c>
     </row>
     <row r="11">
@@ -1510,10 +1510,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1731.237790381144</v>
+        <v>-2323.978848949828</v>
       </c>
       <c r="C11" t="n">
-        <v>2.780674135109495e-35</v>
+        <v>1.955781924445735e-55</v>
       </c>
     </row>
     <row r="12">
@@ -1523,10 +1523,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>21.52954375807661</v>
+        <v>26.03514272915713</v>
       </c>
       <c r="C12" t="n">
-        <v>0.211736016755262</v>
+        <v>0.1553319902665611</v>
       </c>
     </row>
     <row r="13">
@@ -1536,10 +1536,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1206.276563818763</v>
+        <v>-1385.108485946829</v>
       </c>
       <c r="C13" t="n">
-        <v>8.486013947326962e-183</v>
+        <v>8.523412143191507e-212</v>
       </c>
     </row>
     <row r="14">
@@ -1549,10 +1549,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-19.55155480771268</v>
+        <v>-20.47174917748897</v>
       </c>
       <c r="C14" t="n">
-        <v>1.062641876362813e-27</v>
+        <v>7.88047578644924e-27</v>
       </c>
     </row>
     <row r="15">
@@ -1562,10 +1562,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>143.5276631177575</v>
+        <v>164.0088716112463</v>
       </c>
       <c r="C15" t="n">
-        <v>7.601849853780315e-41</v>
+        <v>5.10307953954546e-46</v>
       </c>
     </row>
     <row r="16">
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>365.7095049974536</v>
+        <v>357.5630523142514</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -1588,10 +1588,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0208012903837849</v>
+        <v>-0.01112940130090236</v>
       </c>
       <c r="C17" t="n">
-        <v>3.80503472865775e-09</v>
+        <v>0.002858397604831751</v>
       </c>
     </row>
     <row r="18">
@@ -1601,10 +1601,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-6.599819428970865e-06</v>
+        <v>-4.666415598154401e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.00844376603411651</v>
+        <v>0.08528196832658669</v>
       </c>
     </row>
     <row r="19">
@@ -1614,10 +1614,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-14.44451048727118</v>
+        <v>-14.19897687121607</v>
       </c>
       <c r="C19" t="n">
-        <v>2.598202229441242e-30</v>
+        <v>7.738764583650852e-26</v>
       </c>
     </row>
     <row r="20">
@@ -1627,10 +1627,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>7.471028900236199</v>
+        <v>1.026136715138648</v>
       </c>
       <c r="C20" t="n">
-        <v>2.553849840292246e-07</v>
+        <v>0.5055756644837019</v>
       </c>
     </row>
     <row r="21">
@@ -1640,10 +1640,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3383.798666216394</v>
+        <v>-3238.467747556037</v>
       </c>
       <c r="C21" t="n">
-        <v>4.010140612025101e-54</v>
+        <v>3.645301865379879e-44</v>
       </c>
     </row>
     <row r="22">
@@ -1653,10 +1653,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1476.654249517133</v>
+        <v>-1991.497217116284</v>
       </c>
       <c r="C22" t="n">
-        <v>6.893306050535948e-22</v>
+        <v>9.118684731176602e-34</v>
       </c>
     </row>
   </sheetData>
@@ -1702,10 +1702,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9504.004706765765</v>
+        <v>11108.53408868879</v>
       </c>
       <c r="C2" t="n">
-        <v>6.134615802185355e-253</v>
+        <v>1.231344949885142e-306</v>
       </c>
     </row>
     <row r="3">
@@ -1715,10 +1715,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1231.752947192795</v>
+        <v>-1112.401402627836</v>
       </c>
       <c r="C3" t="n">
-        <v>1.179587901117094e-23</v>
+        <v>1.503882913270819e-17</v>
       </c>
     </row>
     <row r="4">
@@ -1728,10 +1728,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-675.2726819655589</v>
+        <v>-590.8181345105146</v>
       </c>
       <c r="C4" t="n">
-        <v>3.037757544794736e-19</v>
+        <v>1.88871283189855e-13</v>
       </c>
     </row>
     <row r="5">
@@ -1741,10 +1741,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-175.0859654607779</v>
+        <v>32.54258718246882</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01056301864590117</v>
+        <v>0.6558383695960147</v>
       </c>
     </row>
     <row r="6">
@@ -1754,10 +1754,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-59.1015395785281</v>
+        <v>93.83159482911216</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4295209269233371</v>
+        <v>0.2362789371007143</v>
       </c>
     </row>
     <row r="7">
@@ -1767,10 +1767,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-189.3102005249972</v>
+        <v>-86.44533139204083</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0577558654966947</v>
+        <v>0.4101199281257435</v>
       </c>
     </row>
     <row r="8">
@@ -1780,10 +1780,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-407.6711689658852</v>
+        <v>-72.54314184084139</v>
       </c>
       <c r="C8" t="n">
-        <v>4.193310654602646e-09</v>
+        <v>0.3226162461224734</v>
       </c>
     </row>
     <row r="9">
@@ -1793,10 +1793,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1654.132374731478</v>
+        <v>-2136.204074989936</v>
       </c>
       <c r="C9" t="n">
-        <v>3.129870086795752e-37</v>
+        <v>2.258455806129259e-54</v>
       </c>
     </row>
     <row r="10">
@@ -1806,10 +1806,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-971.0283838679406</v>
+        <v>-359.6537391393504</v>
       </c>
       <c r="C10" t="n">
-        <v>5.163763085155186e-14</v>
+        <v>0.008423854406967343</v>
       </c>
     </row>
     <row r="11">
@@ -1819,10 +1819,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1529.25528526474</v>
+        <v>-2135.17327844782</v>
       </c>
       <c r="C11" t="n">
-        <v>6.938560049842389e-28</v>
+        <v>5.552634852008516e-47</v>
       </c>
     </row>
     <row r="12">
@@ -1832,10 +1832,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>28.25769209912677</v>
+        <v>26.81212834849304</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1002352504899713</v>
+        <v>0.1422603156487685</v>
       </c>
     </row>
     <row r="13">
@@ -1845,10 +1845,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1173.632645323415</v>
+        <v>-1398.384144510922</v>
       </c>
       <c r="C13" t="n">
-        <v>7.225183047254564e-174</v>
+        <v>1.253004146546811e-216</v>
       </c>
     </row>
     <row r="14">
@@ -1858,10 +1858,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-19.11636230706807</v>
+        <v>-21.64652780590973</v>
       </c>
       <c r="C14" t="n">
-        <v>1.129765117695437e-26</v>
+        <v>6.985761726004788e-30</v>
       </c>
     </row>
     <row r="15">
@@ -1871,10 +1871,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>149.5144523486144</v>
+        <v>162.8140643957958</v>
       </c>
       <c r="C15" t="n">
-        <v>3.450228830006351e-44</v>
+        <v>1.442167426976532e-45</v>
       </c>
     </row>
     <row r="16">
@@ -1884,7 +1884,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>370.3898550036876</v>
+        <v>358.6857802015351</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -1897,10 +1897,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0194709230836263</v>
+        <v>-0.01524319652483125</v>
       </c>
       <c r="C17" t="n">
-        <v>3.237925555611453e-08</v>
+        <v>4.257759837870722e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1910,10 +1910,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-2.807467202659995e-06</v>
+        <v>-3.855299052876033e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2681671108678023</v>
+        <v>0.1538080058519756</v>
       </c>
     </row>
     <row r="19">
@@ -1923,10 +1923,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-12.3925814608986</v>
+        <v>-13.15238645141663</v>
       </c>
       <c r="C19" t="n">
-        <v>7.574247855760999e-23</v>
+        <v>1.335651240975053e-22</v>
       </c>
     </row>
     <row r="20">
@@ -1936,10 +1936,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10.74984409364992</v>
+        <v>2.599704020062176</v>
       </c>
       <c r="C20" t="n">
-        <v>1.870230660986918e-13</v>
+        <v>0.09210149167142055</v>
       </c>
     </row>
     <row r="21">
@@ -1949,10 +1949,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3262.344528166745</v>
+        <v>-3467.699263848053</v>
       </c>
       <c r="C21" t="n">
-        <v>9.094335656510027e-51</v>
+        <v>1.020615270234315e-50</v>
       </c>
     </row>
     <row r="22">
@@ -1962,10 +1962,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1589.247175753552</v>
+        <v>-2092.841142857649</v>
       </c>
       <c r="C22" t="n">
-        <v>3.46787966484174e-25</v>
+        <v>4.208374313104247e-37</v>
       </c>
     </row>
   </sheetData>
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9699.086272008368</v>
+        <v>11323.49562429782</v>
       </c>
       <c r="C2" t="n">
-        <v>2.126299119751533e-264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2024,10 +2024,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1132.428249879636</v>
+        <v>-1231.084613845567</v>
       </c>
       <c r="C3" t="n">
-        <v>2.03618330661238e-20</v>
+        <v>2.696602046788299e-21</v>
       </c>
     </row>
     <row r="4">
@@ -2037,10 +2037,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-671.6012590993491</v>
+        <v>-735.9702023629134</v>
       </c>
       <c r="C4" t="n">
-        <v>6.2227074324422e-19</v>
+        <v>4.934908567374518e-20</v>
       </c>
     </row>
     <row r="5">
@@ -2050,10 +2050,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-129.770658514416</v>
+        <v>-155.0529918136593</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05921903666618648</v>
+        <v>0.0335181980856356</v>
       </c>
     </row>
     <row r="6">
@@ -2063,10 +2063,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>65.57192863865596</v>
+        <v>35.82645567218469</v>
       </c>
       <c r="C6" t="n">
-        <v>0.380691471343631</v>
+        <v>0.6502074858154919</v>
       </c>
     </row>
     <row r="7">
@@ -2076,10 +2076,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-133.8641449758452</v>
+        <v>-202.5791405017224</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1791941359035943</v>
+        <v>0.05185410846060034</v>
       </c>
     </row>
     <row r="8">
@@ -2089,10 +2089,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-370.600504303209</v>
+        <v>-205.5336465388248</v>
       </c>
       <c r="C8" t="n">
-        <v>9.22020068321039e-08</v>
+        <v>0.005030540482294551</v>
       </c>
     </row>
     <row r="9">
@@ -2102,10 +2102,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1790.941844584777</v>
+        <v>-2172.276848737347</v>
       </c>
       <c r="C9" t="n">
-        <v>3.168039810069552e-43</v>
+        <v>3.398764376581801e-56</v>
       </c>
     </row>
     <row r="10">
@@ -2115,10 +2115,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1072.909042130916</v>
+        <v>-483.0519222359526</v>
       </c>
       <c r="C10" t="n">
-        <v>9.788028776302846e-17</v>
+        <v>0.0003932941799561958</v>
       </c>
     </row>
     <row r="11">
@@ -2128,10 +2128,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1669.336453803191</v>
+        <v>-2203.81004730558</v>
       </c>
       <c r="C11" t="n">
-        <v>8.199729127273861e-33</v>
+        <v>3.586629517548519e-50</v>
       </c>
     </row>
     <row r="12">
@@ -2141,10 +2141,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.450451935672469</v>
+        <v>40.94982910055842</v>
       </c>
       <c r="C12" t="n">
-        <v>0.795614117269978</v>
+        <v>0.02497290861751431</v>
       </c>
     </row>
     <row r="13">
@@ -2154,10 +2154,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1197.493551175097</v>
+        <v>-1371.217280283944</v>
       </c>
       <c r="C13" t="n">
-        <v>2.352842855685726e-180</v>
+        <v>1.094713302134598e-209</v>
       </c>
     </row>
     <row r="14">
@@ -2167,10 +2167,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-20.74823343456319</v>
+        <v>-21.54767393891296</v>
       </c>
       <c r="C14" t="n">
-        <v>5.375567550239298e-31</v>
+        <v>9.201943463927159e-30</v>
       </c>
     </row>
     <row r="15">
@@ -2180,10 +2180,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>151.683938429253</v>
+        <v>175.9887129044791</v>
       </c>
       <c r="C15" t="n">
-        <v>2.625405324485078e-45</v>
+        <v>5.175535265255367e-53</v>
       </c>
     </row>
     <row r="16">
@@ -2193,7 +2193,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>373.8658459275951</v>
+        <v>350.6595976006168</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -2206,10 +2206,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.01942117107749115</v>
+        <v>-0.01170844674898279</v>
       </c>
       <c r="C17" t="n">
-        <v>3.551973280574168e-08</v>
+        <v>0.001627810139935379</v>
       </c>
     </row>
     <row r="18">
@@ -2219,10 +2219,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-4.763102552434075e-06</v>
+        <v>-3.775891650277461e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.05818426861012502</v>
+        <v>0.159608650782976</v>
       </c>
     </row>
     <row r="19">
@@ -2232,10 +2232,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-12.91389866839742</v>
+        <v>-14.69779827371401</v>
       </c>
       <c r="C19" t="n">
-        <v>1.257309579686427e-24</v>
+        <v>6.523795031922052e-28</v>
       </c>
     </row>
     <row r="20">
@@ -2245,10 +2245,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10.2506480428131</v>
+        <v>3.028660874268056</v>
       </c>
       <c r="C20" t="n">
-        <v>1.824022499538158e-12</v>
+        <v>0.04892483167692017</v>
       </c>
     </row>
     <row r="21">
@@ -2258,10 +2258,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3235.306219282032</v>
+        <v>-3318.119239442255</v>
       </c>
       <c r="C21" t="n">
-        <v>8.118222872387138e-50</v>
+        <v>1.213923239146536e-46</v>
       </c>
     </row>
     <row r="22">
@@ -2271,10 +2271,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1461.800727607756</v>
+        <v>-2078.994775111795</v>
       </c>
       <c r="C22" t="n">
-        <v>1.722799631367096e-21</v>
+        <v>7.188343901724091e-37</v>
       </c>
     </row>
   </sheetData>
@@ -2320,10 +2320,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9794.0623624377</v>
+        <v>10957.42578830064</v>
       </c>
       <c r="C2" t="n">
-        <v>2.972591452642468e-269</v>
+        <v>2.007045596937517e-299</v>
       </c>
     </row>
     <row r="3">
@@ -2333,10 +2333,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1165.262104796469</v>
+        <v>-1182.926458753302</v>
       </c>
       <c r="C3" t="n">
-        <v>3.566284676402379e-21</v>
+        <v>8.81084337493556e-20</v>
       </c>
     </row>
     <row r="4">
@@ -2346,10 +2346,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-701.1585684478767</v>
+        <v>-713.3183254129</v>
       </c>
       <c r="C4" t="n">
-        <v>2.305244142377675e-20</v>
+        <v>6.854272115732759e-19</v>
       </c>
     </row>
     <row r="5">
@@ -2359,10 +2359,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-179.5585505119603</v>
+        <v>-65.06023658897521</v>
       </c>
       <c r="C5" t="n">
-        <v>0.009224097814993703</v>
+        <v>0.3728359312823665</v>
       </c>
     </row>
     <row r="6">
@@ -2372,10 +2372,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-6.886340492693563</v>
+        <v>120.4707082974462</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9267439905418035</v>
+        <v>0.1269139805572017</v>
       </c>
     </row>
     <row r="7">
@@ -2385,10 +2385,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-199.6487086638324</v>
+        <v>66.07772173403899</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04619212926914346</v>
+        <v>0.5275398609569233</v>
       </c>
     </row>
     <row r="8">
@@ -2398,10 +2398,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-336.551609979537</v>
+        <v>-124.2704536016469</v>
       </c>
       <c r="C8" t="n">
-        <v>1.278618603478153e-06</v>
+        <v>0.08920677547771816</v>
       </c>
     </row>
     <row r="9">
@@ -2411,10 +2411,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1780.126548094406</v>
+        <v>-2030.115054738794</v>
       </c>
       <c r="C9" t="n">
-        <v>1.152727834800865e-42</v>
+        <v>3.307382614910409e-49</v>
       </c>
     </row>
     <row r="10">
@@ -2424,10 +2424,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1046.435792557013</v>
+        <v>-340.439651526076</v>
       </c>
       <c r="C10" t="n">
-        <v>5.759570349112541e-16</v>
+        <v>0.01256326283907694</v>
       </c>
     </row>
     <row r="11">
@@ -2437,10 +2437,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1651.873053196599</v>
+        <v>-2152.681291248075</v>
       </c>
       <c r="C11" t="n">
-        <v>3.414367269704034e-32</v>
+        <v>9.71605817564732e-48</v>
       </c>
     </row>
     <row r="12">
@@ -2450,10 +2450,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.907883602667383</v>
+        <v>32.37019968451828</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9121052133872127</v>
+        <v>0.0757812986455047</v>
       </c>
     </row>
     <row r="13">
@@ -2463,10 +2463,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1208.716430051062</v>
+        <v>-1367.31061213677</v>
       </c>
       <c r="C13" t="n">
-        <v>1.66930004918222e-182</v>
+        <v>2.002363521140639e-208</v>
       </c>
     </row>
     <row r="14">
@@ -2476,10 +2476,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-18.4354724202105</v>
+        <v>-19.96992954971802</v>
       </c>
       <c r="C14" t="n">
-        <v>1.223803302639652e-24</v>
+        <v>8.054073676233656e-26</v>
       </c>
     </row>
     <row r="15">
@@ -2489,10 +2489,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>148.9827459495725</v>
+        <v>164.9593940188297</v>
       </c>
       <c r="C15" t="n">
-        <v>1.060938814439685e-43</v>
+        <v>6.242170830364092e-47</v>
       </c>
     </row>
     <row r="16">
@@ -2502,7 +2502,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>370.4437693704761</v>
+        <v>356.3242614304127</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -2515,10 +2515,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0196671543725688</v>
+        <v>-0.01208672102820959</v>
       </c>
       <c r="C17" t="n">
-        <v>2.584975685043271e-08</v>
+        <v>0.001141390183770221</v>
       </c>
     </row>
     <row r="18">
@@ -2528,10 +2528,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-5.199769021611962e-06</v>
+        <v>-3.857342082141795e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03980564916190826</v>
+        <v>0.1549582426834339</v>
       </c>
     </row>
     <row r="19">
@@ -2541,10 +2541,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-12.60145861295293</v>
+        <v>-13.71462594609402</v>
       </c>
       <c r="C19" t="n">
-        <v>2.089763849538724e-23</v>
+        <v>1.791877651506753e-24</v>
       </c>
     </row>
     <row r="20">
@@ -2554,10 +2554,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>9.130645283065149</v>
+        <v>2.903751596948024</v>
       </c>
       <c r="C20" t="n">
-        <v>2.878687746555358e-10</v>
+        <v>0.05884929228515778</v>
       </c>
     </row>
     <row r="21">
@@ -2567,10 +2567,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3241.421926192526</v>
+        <v>-3347.897545620197</v>
       </c>
       <c r="C21" t="n">
-        <v>7.341347553522012e-50</v>
+        <v>1.476111862291903e-47</v>
       </c>
     </row>
     <row r="22">
@@ -2580,10 +2580,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1476.647469428249</v>
+        <v>-2029.953129637202</v>
       </c>
       <c r="C22" t="n">
-        <v>8.784543312804281e-22</v>
+        <v>3.721521818471742e-35</v>
       </c>
     </row>
   </sheetData>
@@ -2629,10 +2629,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9936.962380863852</v>
+        <v>11261.11823795387</v>
       </c>
       <c r="C2" t="n">
-        <v>6.136003740584925e-277</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2642,10 +2642,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1231.806383725351</v>
+        <v>-1164.100951635244</v>
       </c>
       <c r="C3" t="n">
-        <v>1.21209140557872e-23</v>
+        <v>5.939829136670214e-19</v>
       </c>
     </row>
     <row r="4">
@@ -2655,10 +2655,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-730.1664467327205</v>
+        <v>-686.8387938068531</v>
       </c>
       <c r="C4" t="n">
-        <v>4.213080954516655e-22</v>
+        <v>1.564596714269924e-17</v>
       </c>
     </row>
     <row r="5">
@@ -2668,10 +2668,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-208.2057382356584</v>
+        <v>-53.32566670052447</v>
       </c>
       <c r="C5" t="n">
-        <v>0.002460622606442307</v>
+        <v>0.4663297537837197</v>
       </c>
     </row>
     <row r="6">
@@ -2681,10 +2681,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.008707806362252768</v>
+        <v>20.47643765053232</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9999071766066399</v>
+        <v>0.7962788718347552</v>
       </c>
     </row>
     <row r="7">
@@ -2694,10 +2694,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-122.1472351440187</v>
+        <v>-68.10783057815159</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2216929671323781</v>
+        <v>0.5158347899799289</v>
       </c>
     </row>
     <row r="8">
@@ -2707,10 +2707,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-347.2894119190956</v>
+        <v>-231.8119604805397</v>
       </c>
       <c r="C8" t="n">
-        <v>5.466658920981087e-07</v>
+        <v>0.001624804794525436</v>
       </c>
     </row>
     <row r="9">
@@ -2720,10 +2720,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1906.588382712493</v>
+        <v>-2216.338046277977</v>
       </c>
       <c r="C9" t="n">
-        <v>2.123554601509805e-48</v>
+        <v>7.826886631454748e-58</v>
       </c>
     </row>
     <row r="10">
@@ -2733,10 +2733,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1136.533332023551</v>
+        <v>-514.0200716192885</v>
       </c>
       <c r="C10" t="n">
-        <v>2.024422823643597e-18</v>
+        <v>0.0001805320920860159</v>
       </c>
     </row>
     <row r="11">
@@ -2746,10 +2746,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1791.575483602951</v>
+        <v>-2328.814049933241</v>
       </c>
       <c r="C11" t="n">
-        <v>2.385459510319993e-37</v>
+        <v>2.90537755086557e-55</v>
       </c>
     </row>
     <row r="12">
@@ -2759,10 +2759,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>20.47397473381995</v>
+        <v>39.68755172641701</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2343022586164185</v>
+        <v>0.03008991892124577</v>
       </c>
     </row>
     <row r="13">
@@ -2772,10 +2772,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1177.230641606485</v>
+        <v>-1371.158904307154</v>
       </c>
       <c r="C13" t="n">
-        <v>5.68695416245091e-174</v>
+        <v>4.226705000930685e-208</v>
       </c>
     </row>
     <row r="14">
@@ -2785,10 +2785,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-19.80517601330437</v>
+        <v>-21.8085706427542</v>
       </c>
       <c r="C14" t="n">
-        <v>2.275380668455561e-28</v>
+        <v>2.786191282729311e-30</v>
       </c>
     </row>
     <row r="15">
@@ -2798,10 +2798,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>150.2378737368616</v>
+        <v>162.4730611093852</v>
       </c>
       <c r="C15" t="n">
-        <v>1.469311466845243e-44</v>
+        <v>3.048586166096628e-45</v>
       </c>
     </row>
     <row r="16">
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>374.3019063171544</v>
+        <v>359.2696811038834</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -2824,10 +2824,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.01941049487005576</v>
+        <v>-0.01225850469713484</v>
       </c>
       <c r="C17" t="n">
-        <v>3.889793233046544e-08</v>
+        <v>0.001003455148062617</v>
       </c>
     </row>
     <row r="18">
@@ -2837,10 +2837,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-4.727501247334884e-06</v>
+        <v>-4.100273273357493e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.06004850284349199</v>
+        <v>0.1295830190915148</v>
       </c>
     </row>
     <row r="19">
@@ -2850,10 +2850,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-12.34991706881706</v>
+        <v>-13.45380154615612</v>
       </c>
       <c r="C19" t="n">
-        <v>1.362929990026952e-22</v>
+        <v>1.627573863759888e-23</v>
       </c>
     </row>
     <row r="20">
@@ -2863,10 +2863,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>9.001970218895401</v>
+        <v>2.723702230342407</v>
       </c>
       <c r="C20" t="n">
-        <v>5.809101170051201e-10</v>
+        <v>0.07571972211451229</v>
       </c>
     </row>
     <row r="21">
@@ -2876,10 +2876,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3248.681837814987</v>
+        <v>-3336.084722242872</v>
       </c>
       <c r="C21" t="n">
-        <v>3.540773406956109e-50</v>
+        <v>4.83374228071487e-47</v>
       </c>
     </row>
     <row r="22">
@@ -2889,10 +2889,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1589.749208461335</v>
+        <v>-1988.76191487816</v>
       </c>
       <c r="C22" t="n">
-        <v>5.280606328785364e-25</v>
+        <v>1.464212995551514e-33</v>
       </c>
     </row>
   </sheetData>
@@ -2938,10 +2938,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9948.477699715615</v>
+        <v>11002.58423222351</v>
       </c>
       <c r="C2" t="n">
-        <v>6.842078733049119e-278</v>
+        <v>9.347707062300088e-300</v>
       </c>
     </row>
     <row r="3">
@@ -2951,10 +2951,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1222.233230098465</v>
+        <v>-1023.163413345411</v>
       </c>
       <c r="C3" t="n">
-        <v>5.036673841677043e-23</v>
+        <v>6.634619292951506e-15</v>
       </c>
     </row>
     <row r="4">
@@ -2964,10 +2964,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-658.7727731104803</v>
+        <v>-640.3943442921848</v>
       </c>
       <c r="C4" t="n">
-        <v>2.767898575316316e-18</v>
+        <v>1.741395433630001e-15</v>
       </c>
     </row>
     <row r="5">
@@ -2977,10 +2977,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-119.6086874145237</v>
+        <v>-0.9743917677456295</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08207071649852857</v>
+        <v>0.9893694015915296</v>
       </c>
     </row>
     <row r="6">
@@ -2990,10 +2990,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27.65750318358573</v>
+        <v>28.30284418024547</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7117735256202375</v>
+        <v>0.7216722189697069</v>
       </c>
     </row>
     <row r="7">
@@ -3003,10 +3003,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-169.9084959449131</v>
+        <v>-126.9973933344853</v>
       </c>
       <c r="C7" t="n">
-        <v>0.08954024082877492</v>
+        <v>0.2260422279812407</v>
       </c>
     </row>
     <row r="8">
@@ -3016,10 +3016,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-355.1543185441984</v>
+        <v>-161.9946947695452</v>
       </c>
       <c r="C8" t="n">
-        <v>3.148883180537497e-07</v>
+        <v>0.02802184467357456</v>
       </c>
     </row>
     <row r="9">
@@ -3029,10 +3029,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1903.467566646196</v>
+        <v>-2004.332456114353</v>
       </c>
       <c r="C9" t="n">
-        <v>3.976301025903471e-48</v>
+        <v>5.507419683267844e-48</v>
       </c>
     </row>
     <row r="10">
@@ -3042,10 +3042,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1112.818892650574</v>
+        <v>-223.1931735209328</v>
       </c>
       <c r="C10" t="n">
-        <v>1.042569833646279e-17</v>
+        <v>0.1025620721929681</v>
       </c>
     </row>
     <row r="11">
@@ -3055,10 +3055,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1741.939407579752</v>
+        <v>-2009.84064297729</v>
       </c>
       <c r="C11" t="n">
-        <v>2.236510928122552e-35</v>
+        <v>7.556492330393665e-42</v>
       </c>
     </row>
     <row r="12">
@@ -3068,10 +3068,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>16.67202879778694</v>
+        <v>29.54215047066098</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3344526515806173</v>
+        <v>0.1070251220222598</v>
       </c>
     </row>
     <row r="13">
@@ -3081,10 +3081,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1193.599221732575</v>
+        <v>-1378.339511418271</v>
       </c>
       <c r="C13" t="n">
-        <v>1.737854747574681e-178</v>
+        <v>5.476202445268156e-210</v>
       </c>
     </row>
     <row r="14">
@@ -3094,10 +3094,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-19.72147503779623</v>
+        <v>-22.72266129628139</v>
       </c>
       <c r="C14" t="n">
-        <v>3.897018919301912e-28</v>
+        <v>1.229257959590328e-32</v>
       </c>
     </row>
     <row r="15">
@@ -3107,10 +3107,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>149.5793451390287</v>
+        <v>154.0893008717019</v>
       </c>
       <c r="C15" t="n">
-        <v>3.40607021522395e-44</v>
+        <v>5.868803125089956e-41</v>
       </c>
     </row>
     <row r="16">
@@ -3120,7 +3120,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>371.3317030348815</v>
+        <v>356.1971199433909</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -3133,10 +3133,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.01786832231427493</v>
+        <v>-0.01646177351392196</v>
       </c>
       <c r="C17" t="n">
-        <v>4.416137319281196e-07</v>
+        <v>1.066657488982354e-05</v>
       </c>
     </row>
     <row r="18">
@@ -3146,10 +3146,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-6.283803788840437e-06</v>
+        <v>-3.304473690466335e-06</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01262594402904619</v>
+        <v>0.2224216834746623</v>
       </c>
     </row>
     <row r="19">
@@ -3159,10 +3159,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-13.08195732741151</v>
+        <v>-12.60547393007116</v>
       </c>
       <c r="C19" t="n">
-        <v>3.347955375165162e-25</v>
+        <v>8.544352062368619e-21</v>
       </c>
     </row>
     <row r="20">
@@ -3172,10 +3172,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>8.655229798546255</v>
+        <v>3.522517178952967</v>
       </c>
       <c r="C20" t="n">
-        <v>2.329948790672791e-09</v>
+        <v>0.02290250650565594</v>
       </c>
     </row>
     <row r="21">
@@ -3185,10 +3185,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3180.458859752187</v>
+        <v>-3440.14077488014</v>
       </c>
       <c r="C21" t="n">
-        <v>4.050054652428327e-48</v>
+        <v>1.595183588552137e-49</v>
       </c>
     </row>
     <row r="22">
@@ -3198,10 +3198,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-1584.177414306186</v>
+        <v>-2096.828618613674</v>
       </c>
       <c r="C22" t="n">
-        <v>7.98922735236574e-25</v>
+        <v>3.392108233407974e-37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>